<commit_message>
Updated structure + requirements.txt
</commit_message>
<xml_diff>
--- a/output/momentum_smooth_by_ticker.xlsx
+++ b/output/momentum_smooth_by_ticker.xlsx
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>92.63346448338974</v>
+        <v>92.63346302724916</v>
       </c>
       <c r="C2" t="n">
         <v>0.6458333333333334</v>
@@ -496,7 +496,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>42.84077947717685</v>
+        <v>42.84077675059142</v>
       </c>
       <c r="C5" t="n">
         <v>0.6666666666666666</v>
@@ -535,7 +535,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15.53264186649847</v>
+        <v>15.53264062687421</v>
       </c>
       <c r="C8" t="n">
         <v>0.6875</v>
@@ -561,7 +561,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>12.43565681127309</v>
+        <v>12.43565955984353</v>
       </c>
       <c r="C10" t="n">
         <v>0.5833333333333334</v>
@@ -587,7 +587,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>9.705081781913707</v>
+        <v>9.705079252010494</v>
       </c>
       <c r="C12" t="n">
         <v>0.5208333333333334</v>
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9.60189821905813</v>
+        <v>9.601898898325526</v>
       </c>
       <c r="C13" t="n">
         <v>0.6458333333333334</v>
@@ -613,7 +613,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>9.356827876140002</v>
+        <v>9.35682786321817</v>
       </c>
       <c r="C14" t="n">
         <v>0.6041666666666666</v>
@@ -626,7 +626,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.414763034286795</v>
+        <v>8.414762914587593</v>
       </c>
       <c r="C15" t="n">
         <v>0.6041666666666666</v>
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>8.151683388322343</v>
+        <v>8.151682336185701</v>
       </c>
       <c r="C17" t="n">
         <v>0.6666666666666666</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>7.936901282477193</v>
+        <v>7.936900656128744</v>
       </c>
       <c r="C19" t="n">
         <v>0.6041666666666666</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6.9924471764247</v>
+        <v>6.992446402545726</v>
       </c>
       <c r="C20" t="n">
         <v>0.625</v>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6.571823013777672</v>
+        <v>6.571825868644099</v>
       </c>
       <c r="C22" t="n">
         <v>0.6666666666666666</v>
@@ -730,7 +730,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6.566208885611168</v>
+        <v>6.566207194026114</v>
       </c>
       <c r="C23" t="n">
         <v>0.6875</v>
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>6.034015418621735</v>
+        <v>6.034014853592867</v>
       </c>
       <c r="C24" t="n">
         <v>0.6666666666666666</v>
@@ -756,7 +756,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5.687129909160141</v>
+        <v>5.68713066551602</v>
       </c>
       <c r="C25" t="n">
         <v>0.5625</v>
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5.286754370404601</v>
+        <v>5.28675487397696</v>
       </c>
       <c r="C26" t="n">
         <v>0.6041666666666666</v>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5.16089583282976</v>
+        <v>5.160895340386044</v>
       </c>
       <c r="C27" t="n">
         <v>0.6458333333333334</v>
@@ -795,7 +795,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5.067332364550539</v>
+        <v>5.06733315275796</v>
       </c>
       <c r="C28" t="n">
         <v>0.6041666666666666</v>
@@ -834,7 +834,7 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>4.839617537727888</v>
+        <v>4.839617186350162</v>
       </c>
       <c r="C31" t="n">
         <v>0.625</v>
@@ -847,7 +847,7 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>4.692913850147103</v>
+        <v>4.692914887970317</v>
       </c>
       <c r="C32" t="n">
         <v>0.6041666666666666</v>
@@ -860,7 +860,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>4.659324585669189</v>
+        <v>4.659323553953545</v>
       </c>
       <c r="C33" t="n">
         <v>0.6041666666666666</v>
@@ -873,7 +873,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>4.575143801258394</v>
+        <v>4.575142600605631</v>
       </c>
       <c r="C34" t="n">
         <v>0.5833333333333334</v>
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>4.562870005832982</v>
+        <v>4.5628696536799</v>
       </c>
       <c r="C35" t="n">
         <v>0.6041666666666666</v>
@@ -899,7 +899,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>4.466611995798737</v>
+        <v>4.46661197934056</v>
       </c>
       <c r="C36" t="n">
         <v>0.5416666666666666</v>
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>4.23172317013896</v>
+        <v>4.231722796011653</v>
       </c>
       <c r="C37" t="n">
         <v>0.6458333333333334</v>
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4.168415381546968</v>
+        <v>4.168414105075744</v>
       </c>
       <c r="C38" t="n">
         <v>0.5625</v>
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>3.778205617191114</v>
+        <v>3.778205279787008</v>
       </c>
       <c r="C40" t="n">
         <v>0.5833333333333334</v>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>3.763658769023674</v>
+        <v>3.763658739142673</v>
       </c>
       <c r="C41" t="n">
         <v>0.5833333333333334</v>
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3.469594996253949</v>
+        <v>3.469595847032819</v>
       </c>
       <c r="C44" t="n">
         <v>0.5416666666666666</v>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>3.412546422055625</v>
+        <v>3.412545476923442</v>
       </c>
       <c r="C45" t="n">
         <v>0.6041666666666666</v>
@@ -1042,7 +1042,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>3.35528462117768</v>
+        <v>3.355284586582792</v>
       </c>
       <c r="C47" t="n">
         <v>0.6041666666666666</v>
@@ -1081,7 +1081,7 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>3.260030181997773</v>
+        <v>3.26003050342412</v>
       </c>
       <c r="C50" t="n">
         <v>0.6458333333333334</v>
@@ -1094,7 +1094,7 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>3.239130642433328</v>
+        <v>3.239129421237521</v>
       </c>
       <c r="C51" t="n">
         <v>0.625</v>
@@ -1107,7 +1107,7 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>3.216650041846996</v>
+        <v>3.216650041846994</v>
       </c>
       <c r="C52" t="n">
         <v>0.5833333333333334</v>
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>3.118165197512792</v>
+        <v>3.118165203510343</v>
       </c>
       <c r="C53" t="n">
         <v>0.5625</v>
@@ -1133,7 +1133,7 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3.114376676334385</v>
+        <v>3.114376380489734</v>
       </c>
       <c r="C54" t="n">
         <v>0.6666666666666666</v>
@@ -1146,7 +1146,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>3.066547977384599</v>
+        <v>3.06654706182044</v>
       </c>
       <c r="C55" t="n">
         <v>0.6041666666666666</v>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>3.060619997529298</v>
+        <v>3.060619487787939</v>
       </c>
       <c r="C56" t="n">
         <v>0.625</v>
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>3.011913931034412</v>
+        <v>3.011912675965313</v>
       </c>
       <c r="C57" t="n">
         <v>0.5416666666666666</v>
@@ -1211,7 +1211,7 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>2.975416882750367</v>
+        <v>2.97541757939047</v>
       </c>
       <c r="C60" t="n">
         <v>0.625</v>
@@ -1224,7 +1224,7 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>2.946126684867365</v>
+        <v>2.946126354505936</v>
       </c>
       <c r="C61" t="n">
         <v>0.625</v>
@@ -1237,7 +1237,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2.926499133723486</v>
+        <v>2.92649912557744</v>
       </c>
       <c r="C62" t="n">
         <v>0.5625</v>
@@ -1250,7 +1250,7 @@
         </is>
       </c>
       <c r="B63" t="n">
-        <v>2.894403610706259</v>
+        <v>2.894403617360329</v>
       </c>
       <c r="C63" t="n">
         <v>0.5416666666666666</v>
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>2.841944977942299</v>
+        <v>2.841944952136562</v>
       </c>
       <c r="C66" t="n">
         <v>0.625</v>
@@ -1302,7 +1302,7 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>2.838625648236817</v>
+        <v>2.838625648236818</v>
       </c>
       <c r="C67" t="n">
         <v>0.625</v>
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>2.774565574397279</v>
+        <v>2.774565926684331</v>
       </c>
       <c r="C68" t="n">
         <v>0.6875</v>
@@ -1328,7 +1328,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>2.748767712557672</v>
+        <v>2.748768996308808</v>
       </c>
       <c r="C69" t="n">
         <v>0.6458333333333334</v>
@@ -1367,7 +1367,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>2.712854778220031</v>
+        <v>2.712854779358288</v>
       </c>
       <c r="C72" t="n">
         <v>0.6041666666666666</v>
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>2.70994933947732</v>
+        <v>2.709949331422547</v>
       </c>
       <c r="C73" t="n">
         <v>0.625</v>
@@ -1393,7 +1393,7 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>2.689374466676085</v>
+        <v>2.689374143842502</v>
       </c>
       <c r="C74" t="n">
         <v>0.6666666666666666</v>
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>2.66017255477937</v>
+        <v>2.660172214746918</v>
       </c>
       <c r="C75" t="n">
         <v>0.625</v>
@@ -1419,7 +1419,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>2.65411818464277</v>
+        <v>2.654118618070543</v>
       </c>
       <c r="C76" t="n">
         <v>0.6458333333333334</v>
@@ -1445,7 +1445,7 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>2.595319407353918</v>
+        <v>2.59531965407186</v>
       </c>
       <c r="C78" t="n">
         <v>0.6041666666666666</v>
@@ -1458,7 +1458,7 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>2.586965357467902</v>
+        <v>2.586965355333104</v>
       </c>
       <c r="C79" t="n">
         <v>0.6875</v>
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>2.567285293132846</v>
+        <v>2.567285060357936</v>
       </c>
       <c r="C80" t="n">
         <v>0.6458333333333334</v>
@@ -1484,7 +1484,7 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>2.518028108914504</v>
+        <v>2.518027725227034</v>
       </c>
       <c r="C81" t="n">
         <v>0.6041666666666666</v>
@@ -1523,7 +1523,7 @@
         </is>
       </c>
       <c r="B84" t="n">
-        <v>2.454789843007543</v>
+        <v>2.454789610928609</v>
       </c>
       <c r="C84" t="n">
         <v>0.5208333333333334</v>
@@ -1536,7 +1536,7 @@
         </is>
       </c>
       <c r="B85" t="n">
-        <v>2.451091215399427</v>
+        <v>2.451091208405587</v>
       </c>
       <c r="C85" t="n">
         <v>0.6041666666666666</v>
@@ -1562,7 +1562,7 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>2.415531522976703</v>
+        <v>2.415531895183964</v>
       </c>
       <c r="C87" t="n">
         <v>0.6458333333333334</v>
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>2.343933205107429</v>
+        <v>2.343933461899772</v>
       </c>
       <c r="C88" t="n">
         <v>0.6041666666666666</v>
@@ -1588,7 +1588,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>2.316392604936374</v>
+        <v>2.316392604936375</v>
       </c>
       <c r="C89" t="n">
         <v>0.5416666666666666</v>
@@ -1601,7 +1601,7 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>2.301850035614402</v>
+        <v>2.30185073554353</v>
       </c>
       <c r="C90" t="n">
         <v>0.6041666666666666</v>
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>2.291407707383676</v>
+        <v>2.291407436417433</v>
       </c>
       <c r="C91" t="n">
         <v>0.625</v>
@@ -1666,7 +1666,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>2.233662854384801</v>
+        <v>2.233663180059532</v>
       </c>
       <c r="C95" t="n">
         <v>0.6041666666666666</v>
@@ -1679,7 +1679,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>2.221084904352429</v>
+        <v>2.221085515437635</v>
       </c>
       <c r="C96" t="n">
         <v>0.6041666666666666</v>
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>2.216285099018717</v>
+        <v>2.216285449955963</v>
       </c>
       <c r="C97" t="n">
         <v>0.6666666666666666</v>
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>2.194184686901303</v>
+        <v>2.194184696195059</v>
       </c>
       <c r="C98" t="n">
         <v>0.5833333333333334</v>
@@ -1718,7 +1718,7 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>2.112523998742271</v>
+        <v>2.112523453651214</v>
       </c>
       <c r="C99" t="n">
         <v>0.5625</v>
@@ -1731,7 +1731,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>2.097835535805434</v>
+        <v>2.097835766892362</v>
       </c>
       <c r="C100" t="n">
         <v>0.6666666666666666</v>
@@ -1744,7 +1744,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2.089731690694055</v>
+        <v>2.089731911889424</v>
       </c>
       <c r="C101" t="n">
         <v>0.5833333333333334</v>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>2.047077559488958</v>
+        <v>2.047078261950399</v>
       </c>
       <c r="C102" t="n">
         <v>0.6041666666666666</v>
@@ -1770,7 +1770,7 @@
         </is>
       </c>
       <c r="B103" t="n">
-        <v>2.008476822168785</v>
+        <v>2.008476245977106</v>
       </c>
       <c r="C103" t="n">
         <v>0.5625</v>
@@ -1796,7 +1796,7 @@
         </is>
       </c>
       <c r="B105" t="n">
-        <v>1.991718874315473</v>
+        <v>1.991718879912992</v>
       </c>
       <c r="C105" t="n">
         <v>0.625</v>
@@ -1809,7 +1809,7 @@
         </is>
       </c>
       <c r="B106" t="n">
-        <v>1.930945792149099</v>
+        <v>1.930945398024651</v>
       </c>
       <c r="C106" t="n">
         <v>0.5833333333333334</v>
@@ -1822,7 +1822,7 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1.922228373510421</v>
+        <v>1.922228373510422</v>
       </c>
       <c r="C107" t="n">
         <v>0.5833333333333334</v>
@@ -1835,7 +1835,7 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1.893531277388548</v>
+        <v>1.893530987857648</v>
       </c>
       <c r="C108" t="n">
         <v>0.5625</v>
@@ -1848,7 +1848,7 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1.885988861783735</v>
+        <v>1.885989337037252</v>
       </c>
       <c r="C109" t="n">
         <v>0.4583333333333333</v>
@@ -1874,7 +1874,7 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>1.789380998199179</v>
+        <v>1.78938077885797</v>
       </c>
       <c r="C111" t="n">
         <v>0.625</v>
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>1.766971284608674</v>
+        <v>1.766970696945462</v>
       </c>
       <c r="C112" t="n">
         <v>0.5833333333333334</v>
@@ -1900,7 +1900,7 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>1.76378908759661</v>
+        <v>1.763789365200779</v>
       </c>
       <c r="C113" t="n">
         <v>0.5208333333333334</v>
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>1.746964293423229</v>
+        <v>1.746964045296283</v>
       </c>
       <c r="C114" t="n">
         <v>0.5625</v>
@@ -1939,7 +1939,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>1.724242980689467</v>
+        <v>1.724243228015409</v>
       </c>
       <c r="C116" t="n">
         <v>0.625</v>
@@ -1952,7 +1952,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>1.667039884787495</v>
+        <v>1.667040106567519</v>
       </c>
       <c r="C117" t="n">
         <v>0.6041666666666666</v>
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>1.660509108354944</v>
+        <v>1.660508800239641</v>
       </c>
       <c r="C118" t="n">
         <v>0.5625</v>
@@ -1978,7 +1978,7 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>1.647432466546051</v>
+        <v>1.647433012923062</v>
       </c>
       <c r="C119" t="n">
         <v>0.4791666666666667</v>
@@ -1991,7 +1991,7 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>1.611253484258758</v>
+        <v>1.611253952106183</v>
       </c>
       <c r="C120" t="n">
         <v>0.4791666666666667</v>
@@ -2004,7 +2004,7 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>1.600478081818904</v>
+        <v>1.600477876497098</v>
       </c>
       <c r="C121" t="n">
         <v>0.5833333333333334</v>
@@ -2017,7 +2017,7 @@
         </is>
       </c>
       <c r="B122" t="n">
-        <v>1.561916447405027</v>
+        <v>1.561916445032482</v>
       </c>
       <c r="C122" t="n">
         <v>0.5208333333333334</v>
@@ -2043,7 +2043,7 @@
         </is>
       </c>
       <c r="B124" t="n">
-        <v>1.489447874224915</v>
+        <v>1.489447537219023</v>
       </c>
       <c r="C124" t="n">
         <v>0.625</v>
@@ -2056,7 +2056,7 @@
         </is>
       </c>
       <c r="B125" t="n">
-        <v>1.475107871234404</v>
+        <v>1.475108604571104</v>
       </c>
       <c r="C125" t="n">
         <v>0.5416666666666666</v>
@@ -2069,7 +2069,7 @@
         </is>
       </c>
       <c r="B126" t="n">
-        <v>1.469813315791746</v>
+        <v>1.469813315791745</v>
       </c>
       <c r="C126" t="n">
         <v>0.5625</v>
@@ -2121,7 +2121,7 @@
         </is>
       </c>
       <c r="B130" t="n">
-        <v>1.463870038878861</v>
+        <v>1.463870038878862</v>
       </c>
       <c r="C130" t="n">
         <v>0.5625</v>
@@ -2147,7 +2147,7 @@
         </is>
       </c>
       <c r="B132" t="n">
-        <v>1.434746350624043</v>
+        <v>1.434746344747055</v>
       </c>
       <c r="C132" t="n">
         <v>0.6875</v>
@@ -2160,7 +2160,7 @@
         </is>
       </c>
       <c r="B133" t="n">
-        <v>1.427596832309038</v>
+        <v>1.427597211031491</v>
       </c>
       <c r="C133" t="n">
         <v>0.5833333333333334</v>
@@ -2186,7 +2186,7 @@
         </is>
       </c>
       <c r="B135" t="n">
-        <v>1.37767944909085</v>
+        <v>1.377679434924621</v>
       </c>
       <c r="C135" t="n">
         <v>0.5416666666666666</v>
@@ -2212,7 +2212,7 @@
         </is>
       </c>
       <c r="B137" t="n">
-        <v>1.372049694192455</v>
+        <v>1.372049702917465</v>
       </c>
       <c r="C137" t="n">
         <v>0.6041666666666666</v>
@@ -2251,7 +2251,7 @@
         </is>
       </c>
       <c r="B140" t="n">
-        <v>1.344686019134881</v>
+        <v>1.344686206456654</v>
       </c>
       <c r="C140" t="n">
         <v>0.6041666666666666</v>
@@ -2264,7 +2264,7 @@
         </is>
       </c>
       <c r="B141" t="n">
-        <v>1.322031013788382</v>
+        <v>1.322031169872749</v>
       </c>
       <c r="C141" t="n">
         <v>0.6458333333333334</v>
@@ -2277,7 +2277,7 @@
         </is>
       </c>
       <c r="B142" t="n">
-        <v>1.313213681272581</v>
+        <v>1.313213221201127</v>
       </c>
       <c r="C142" t="n">
         <v>0.5416666666666666</v>
@@ -2290,7 +2290,7 @@
         </is>
       </c>
       <c r="B143" t="n">
-        <v>1.311336674651464</v>
+        <v>1.311336495943721</v>
       </c>
       <c r="C143" t="n">
         <v>0.625</v>
@@ -2303,7 +2303,7 @@
         </is>
       </c>
       <c r="B144" t="n">
-        <v>1.302469493806706</v>
+        <v>1.302469003375489</v>
       </c>
       <c r="C144" t="n">
         <v>0.5416666666666666</v>
@@ -2316,7 +2316,7 @@
         </is>
       </c>
       <c r="B145" t="n">
-        <v>1.299128371420337</v>
+        <v>1.299128109703094</v>
       </c>
       <c r="C145" t="n">
         <v>0.5625</v>
@@ -2329,7 +2329,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>1.29250005693207</v>
+        <v>1.292500056932071</v>
       </c>
       <c r="C146" t="n">
         <v>0.5416666666666666</v>
@@ -2342,7 +2342,7 @@
         </is>
       </c>
       <c r="B147" t="n">
-        <v>1.290190927097735</v>
+        <v>1.290190524666303</v>
       </c>
       <c r="C147" t="n">
         <v>0.5208333333333334</v>
@@ -2355,7 +2355,7 @@
         </is>
       </c>
       <c r="B148" t="n">
-        <v>1.267177116645707</v>
+        <v>1.26717727393994</v>
       </c>
       <c r="C148" t="n">
         <v>0.5208333333333334</v>
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>1.204883096453569</v>
+        <v>1.204882848550921</v>
       </c>
       <c r="C152" t="n">
         <v>0.5833333333333334</v>
@@ -2420,7 +2420,7 @@
         </is>
       </c>
       <c r="B153" t="n">
-        <v>1.204099308294447</v>
+        <v>1.204099308294445</v>
       </c>
       <c r="C153" t="n">
         <v>0.5833333333333334</v>
@@ -2433,7 +2433,7 @@
         </is>
       </c>
       <c r="B154" t="n">
-        <v>1.192194601814987</v>
+        <v>1.192194119699807</v>
       </c>
       <c r="C154" t="n">
         <v>0.5833333333333334</v>
@@ -2446,7 +2446,7 @@
         </is>
       </c>
       <c r="B155" t="n">
-        <v>1.15834973115057</v>
+        <v>1.158349451145265</v>
       </c>
       <c r="C155" t="n">
         <v>0.5416666666666666</v>
@@ -2472,7 +2472,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>1.111651967316979</v>
+        <v>1.111651611318714</v>
       </c>
       <c r="C157" t="n">
         <v>0.5833333333333334</v>
@@ -2485,7 +2485,7 @@
         </is>
       </c>
       <c r="B158" t="n">
-        <v>1.108259273533796</v>
+        <v>1.108259537039782</v>
       </c>
       <c r="C158" t="n">
         <v>0.4791666666666667</v>
@@ -2498,7 +2498,7 @@
         </is>
       </c>
       <c r="B159" t="n">
-        <v>1.10760687315865</v>
+        <v>1.107607309247105</v>
       </c>
       <c r="C159" t="n">
         <v>0.5416666666666666</v>
@@ -2524,7 +2524,7 @@
         </is>
       </c>
       <c r="B161" t="n">
-        <v>1.09127055981524</v>
+        <v>1.091270715252821</v>
       </c>
       <c r="C161" t="n">
         <v>0.6041666666666666</v>
@@ -2537,7 +2537,7 @@
         </is>
       </c>
       <c r="B162" t="n">
-        <v>1.090591769618897</v>
+        <v>1.090591556147086</v>
       </c>
       <c r="C162" t="n">
         <v>0.5416666666666666</v>
@@ -2550,7 +2550,7 @@
         </is>
       </c>
       <c r="B163" t="n">
-        <v>1.083278611255465</v>
+        <v>1.083278614403981</v>
       </c>
       <c r="C163" t="n">
         <v>0.5833333333333334</v>
@@ -2563,7 +2563,7 @@
         </is>
       </c>
       <c r="B164" t="n">
-        <v>1.072776185508686</v>
+        <v>1.072776433878185</v>
       </c>
       <c r="C164" t="n">
         <v>0.5833333333333334</v>
@@ -2576,7 +2576,7 @@
         </is>
       </c>
       <c r="B165" t="n">
-        <v>1.058054289417227</v>
+        <v>1.058053945688703</v>
       </c>
       <c r="C165" t="n">
         <v>0.5416666666666666</v>
@@ -2589,7 +2589,7 @@
         </is>
       </c>
       <c r="B166" t="n">
-        <v>1.053560546406793</v>
+        <v>1.05356034140662</v>
       </c>
       <c r="C166" t="n">
         <v>0.4791666666666667</v>
@@ -2615,7 +2615,7 @@
         </is>
       </c>
       <c r="B168" t="n">
-        <v>1.043047433767261</v>
+        <v>1.043047262627146</v>
       </c>
       <c r="C168" t="n">
         <v>0.5416666666666666</v>
@@ -2628,7 +2628,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>1.034428772249392</v>
+        <v>1.03442850708704</v>
       </c>
       <c r="C169" t="n">
         <v>0.5208333333333334</v>
@@ -2641,7 +2641,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>1.029427367617578</v>
+        <v>1.029427358713172</v>
       </c>
       <c r="C170" t="n">
         <v>0.5625</v>
@@ -2654,7 +2654,7 @@
         </is>
       </c>
       <c r="B171" t="n">
-        <v>1.018514378145677</v>
+        <v>1.018514558208603</v>
       </c>
       <c r="C171" t="n">
         <v>0.5625</v>
@@ -2667,7 +2667,7 @@
         </is>
       </c>
       <c r="B172" t="n">
-        <v>0.9983587531276319</v>
+        <v>0.9983586381443139</v>
       </c>
       <c r="C172" t="n">
         <v>0.5625</v>
@@ -2680,7 +2680,7 @@
         </is>
       </c>
       <c r="B173" t="n">
-        <v>0.9623013156942211</v>
+        <v>0.9623014354114898</v>
       </c>
       <c r="C173" t="n">
         <v>0.5208333333333334</v>
@@ -2693,7 +2693,7 @@
         </is>
       </c>
       <c r="B174" t="n">
-        <v>0.9235999506996455</v>
+        <v>0.9235999531706387</v>
       </c>
       <c r="C174" t="n">
         <v>0.4791666666666667</v>
@@ -2719,7 +2719,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>0.8954486650516242</v>
+        <v>0.8954483000018567</v>
       </c>
       <c r="C176" t="n">
         <v>0.5625</v>
@@ -2732,7 +2732,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>0.8759652495942882</v>
+        <v>0.8759655133147732</v>
       </c>
       <c r="C177" t="n">
         <v>0.5208333333333334</v>
@@ -2745,7 +2745,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>0.8751063150979443</v>
+        <v>0.8751064763858469</v>
       </c>
       <c r="C178" t="n">
         <v>0.625</v>
@@ -2758,7 +2758,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>0.8714703249461759</v>
+        <v>0.8714701936174414</v>
       </c>
       <c r="C179" t="n">
         <v>0.6041666666666666</v>
@@ -2784,7 +2784,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>0.8595373449277679</v>
+        <v>0.8595371828096234</v>
       </c>
       <c r="C181" t="n">
         <v>0.5</v>
@@ -2797,7 +2797,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>0.8550564872752091</v>
+        <v>0.8550569037752429</v>
       </c>
       <c r="C182" t="n">
         <v>0.5416666666666666</v>
@@ -2810,7 +2810,7 @@
         </is>
       </c>
       <c r="B183" t="n">
-        <v>0.8483611297147355</v>
+        <v>0.8483612458548311</v>
       </c>
       <c r="C183" t="n">
         <v>0.6041666666666666</v>
@@ -2823,7 +2823,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>0.8398103073508518</v>
+        <v>0.8398101085288703</v>
       </c>
       <c r="C184" t="n">
         <v>0.4583333333333333</v>
@@ -2836,7 +2836,7 @@
         </is>
       </c>
       <c r="B185" t="n">
-        <v>0.8385901592464071</v>
+        <v>0.8385908039653418</v>
       </c>
       <c r="C185" t="n">
         <v>0.6041666666666666</v>
@@ -2849,7 +2849,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>0.8278298480551189</v>
+        <v>0.8278300921542421</v>
       </c>
       <c r="C186" t="n">
         <v>0.5625</v>
@@ -2862,7 +2862,7 @@
         </is>
       </c>
       <c r="B187" t="n">
-        <v>0.8217751536327453</v>
+        <v>0.8217749879939491</v>
       </c>
       <c r="C187" t="n">
         <v>0.5833333333333334</v>
@@ -2875,7 +2875,7 @@
         </is>
       </c>
       <c r="B188" t="n">
-        <v>0.8046954097247776</v>
+        <v>0.8046954037073029</v>
       </c>
       <c r="C188" t="n">
         <v>0.5208333333333334</v>
@@ -2901,7 +2901,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>0.8007571667368716</v>
+        <v>0.8007574308776886</v>
       </c>
       <c r="C190" t="n">
         <v>0.6041666666666666</v>
@@ -2914,7 +2914,7 @@
         </is>
       </c>
       <c r="B191" t="n">
-        <v>0.7955936152598766</v>
+        <v>0.7955937397432828</v>
       </c>
       <c r="C191" t="n">
         <v>0.5</v>
@@ -2927,7 +2927,7 @@
         </is>
       </c>
       <c r="B192" t="n">
-        <v>0.7903349591847126</v>
+        <v>0.7903348469371625</v>
       </c>
       <c r="C192" t="n">
         <v>0.4791666666666667</v>
@@ -2940,7 +2940,7 @@
         </is>
       </c>
       <c r="B193" t="n">
-        <v>0.786182491816966</v>
+        <v>0.7861827604560945</v>
       </c>
       <c r="C193" t="n">
         <v>0.4791666666666667</v>
@@ -2953,7 +2953,7 @@
         </is>
       </c>
       <c r="B194" t="n">
-        <v>0.7745423308148922</v>
+        <v>0.7745421897245286</v>
       </c>
       <c r="C194" t="n">
         <v>0.5833333333333334</v>
@@ -2966,7 +2966,7 @@
         </is>
       </c>
       <c r="B195" t="n">
-        <v>0.7725204662314289</v>
+        <v>0.7725203490938588</v>
       </c>
       <c r="C195" t="n">
         <v>0.5208333333333334</v>
@@ -2979,7 +2979,7 @@
         </is>
       </c>
       <c r="B196" t="n">
-        <v>0.7589112674035805</v>
+        <v>0.758911411318778</v>
       </c>
       <c r="C196" t="n">
         <v>0.5625</v>
@@ -2992,7 +2992,7 @@
         </is>
       </c>
       <c r="B197" t="n">
-        <v>0.7574362402563493</v>
+        <v>0.7574361063953556</v>
       </c>
       <c r="C197" t="n">
         <v>0.5416666666666666</v>
@@ -3005,7 +3005,7 @@
         </is>
       </c>
       <c r="B198" t="n">
-        <v>0.7545537510014046</v>
+        <v>0.7545537546753989</v>
       </c>
       <c r="C198" t="n">
         <v>0.5833333333333334</v>
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="B199" t="n">
-        <v>0.7452977234220635</v>
+        <v>0.7452978334284768</v>
       </c>
       <c r="C199" t="n">
         <v>0.6458333333333334</v>
@@ -3044,7 +3044,7 @@
         </is>
       </c>
       <c r="B201" t="n">
-        <v>0.7197138841977895</v>
+        <v>0.7197136380250104</v>
       </c>
       <c r="C201" t="n">
         <v>0.6041666666666666</v>
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>0.7106653169124546</v>
+        <v>0.7106650354894788</v>
       </c>
       <c r="C202" t="n">
         <v>0.5833333333333334</v>
@@ -3070,7 +3070,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>0.7028344220872833</v>
+        <v>0.7028347900980443</v>
       </c>
       <c r="C203" t="n">
         <v>0.5625</v>
@@ -3083,7 +3083,7 @@
         </is>
       </c>
       <c r="B204" t="n">
-        <v>0.7004379462371344</v>
+        <v>0.7004378069591743</v>
       </c>
       <c r="C204" t="n">
         <v>0.5625</v>
@@ -3096,7 +3096,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>0.6936793417759657</v>
+        <v>0.6936789456836414</v>
       </c>
       <c r="C205" t="n">
         <v>0.5833333333333334</v>
@@ -3135,7 +3135,7 @@
         </is>
       </c>
       <c r="B208" t="n">
-        <v>0.6890240711934672</v>
+        <v>0.6890239296731819</v>
       </c>
       <c r="C208" t="n">
         <v>0.5833333333333334</v>
@@ -3148,7 +3148,7 @@
         </is>
       </c>
       <c r="B209" t="n">
-        <v>0.6866652816039824</v>
+        <v>0.6866652851212385</v>
       </c>
       <c r="C209" t="n">
         <v>0.5833333333333334</v>
@@ -3174,7 +3174,7 @@
         </is>
       </c>
       <c r="B211" t="n">
-        <v>0.6798790879389534</v>
+        <v>0.6798792204369881</v>
       </c>
       <c r="C211" t="n">
         <v>0.5833333333333334</v>
@@ -3187,7 +3187,7 @@
         </is>
       </c>
       <c r="B212" t="n">
-        <v>0.6787358985200656</v>
+        <v>0.6787359032300044</v>
       </c>
       <c r="C212" t="n">
         <v>0.5208333333333334</v>
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="B213" t="n">
-        <v>0.6768372311264474</v>
+        <v>0.6768378753654225</v>
       </c>
       <c r="C213" t="n">
         <v>0.5625</v>
@@ -3213,7 +3213,7 @@
         </is>
       </c>
       <c r="B214" t="n">
-        <v>0.6389280632731669</v>
+        <v>0.6389280621662454</v>
       </c>
       <c r="C214" t="n">
         <v>0.5625</v>
@@ -3239,7 +3239,7 @@
         </is>
       </c>
       <c r="B216" t="n">
-        <v>0.6341781752502718</v>
+        <v>0.6341787096152547</v>
       </c>
       <c r="C216" t="n">
         <v>0.5208333333333334</v>
@@ -3252,7 +3252,7 @@
         </is>
       </c>
       <c r="B217" t="n">
-        <v>0.6333612178670294</v>
+        <v>0.633360992879993</v>
       </c>
       <c r="C217" t="n">
         <v>0.5833333333333334</v>
@@ -3265,7 +3265,7 @@
         </is>
       </c>
       <c r="B218" t="n">
-        <v>0.6300224508384999</v>
+        <v>0.6300223363300546</v>
       </c>
       <c r="C218" t="n">
         <v>0.5416666666666666</v>
@@ -3291,7 +3291,7 @@
         </is>
       </c>
       <c r="B220" t="n">
-        <v>0.5876637375816882</v>
+        <v>0.5876637373738192</v>
       </c>
       <c r="C220" t="n">
         <v>0.375</v>
@@ -3304,7 +3304,7 @@
         </is>
       </c>
       <c r="B221" t="n">
-        <v>0.5818979711833967</v>
+        <v>0.5818979711833969</v>
       </c>
       <c r="C221" t="n">
         <v>0.5208333333333334</v>
@@ -3317,7 +3317,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>0.5795287093428054</v>
+        <v>0.5795285175273892</v>
       </c>
       <c r="C222" t="n">
         <v>0.6666666666666666</v>
@@ -3343,7 +3343,7 @@
         </is>
       </c>
       <c r="B224" t="n">
-        <v>0.5733423007057021</v>
+        <v>0.5733420035822487</v>
       </c>
       <c r="C224" t="n">
         <v>0.5416666666666666</v>
@@ -3356,7 +3356,7 @@
         </is>
       </c>
       <c r="B225" t="n">
-        <v>0.5632761763079086</v>
+        <v>0.5632760806562276</v>
       </c>
       <c r="C225" t="n">
         <v>0.5208333333333334</v>
@@ -3369,7 +3369,7 @@
         </is>
       </c>
       <c r="B226" t="n">
-        <v>0.5598879391586897</v>
+        <v>0.5598880367114436</v>
       </c>
       <c r="C226" t="n">
         <v>0.4791666666666667</v>
@@ -3382,7 +3382,7 @@
         </is>
       </c>
       <c r="B227" t="n">
-        <v>0.5526442114364889</v>
+        <v>0.5526442114364882</v>
       </c>
       <c r="C227" t="n">
         <v>0.5208333333333334</v>
@@ -3395,7 +3395,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>0.5513517962209968</v>
+        <v>0.5513519547465764</v>
       </c>
       <c r="C228" t="n">
         <v>0.5208333333333334</v>
@@ -3434,7 +3434,7 @@
         </is>
       </c>
       <c r="B231" t="n">
-        <v>0.5097360134973667</v>
+        <v>0.5097357844125672</v>
       </c>
       <c r="C231" t="n">
         <v>0.5625</v>
@@ -3447,7 +3447,7 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>0.5047735487892619</v>
+        <v>0.5047733772275593</v>
       </c>
       <c r="C232" t="n">
         <v>0.5</v>
@@ -3460,7 +3460,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>0.4951537378571054</v>
+        <v>0.4951537376952304</v>
       </c>
       <c r="C233" t="n">
         <v>0.5208333333333334</v>
@@ -3473,7 +3473,7 @@
         </is>
       </c>
       <c r="B234" t="n">
-        <v>0.4943449902561454</v>
+        <v>0.4943450952938013</v>
       </c>
       <c r="C234" t="n">
         <v>0.5625</v>
@@ -3486,7 +3486,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>0.4870089308247347</v>
+        <v>0.4870089310663592</v>
       </c>
       <c r="C235" t="n">
         <v>0.5</v>
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="B237" t="n">
-        <v>0.4816547346245581</v>
+        <v>0.4816548426561302</v>
       </c>
       <c r="C237" t="n">
         <v>0.5625</v>
@@ -3525,7 +3525,7 @@
         </is>
       </c>
       <c r="B238" t="n">
-        <v>0.4779408059626178</v>
+        <v>0.4779409436192352</v>
       </c>
       <c r="C238" t="n">
         <v>0.5416666666666666</v>
@@ -3538,7 +3538,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>0.4758401500001033</v>
+        <v>0.4758402559534869</v>
       </c>
       <c r="C239" t="n">
         <v>0.5833333333333334</v>
@@ -3551,7 +3551,7 @@
         </is>
       </c>
       <c r="B240" t="n">
-        <v>0.4712346974414876</v>
+        <v>0.4712348616752033</v>
       </c>
       <c r="C240" t="n">
         <v>0.5416666666666666</v>
@@ -3577,7 +3577,7 @@
         </is>
       </c>
       <c r="B242" t="n">
-        <v>0.4481255570230822</v>
+        <v>0.4481257110659318</v>
       </c>
       <c r="C242" t="n">
         <v>0.5625</v>
@@ -3590,7 +3590,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>0.4467494784663872</v>
+        <v>0.446749365910736</v>
       </c>
       <c r="C243" t="n">
         <v>0.625</v>
@@ -3616,7 +3616,7 @@
         </is>
       </c>
       <c r="B245" t="n">
-        <v>0.4078132193207367</v>
+        <v>0.4078129354307558</v>
       </c>
       <c r="C245" t="n">
         <v>0.5625</v>
@@ -3629,7 +3629,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>0.4074558914825732</v>
+        <v>0.4074558845012255</v>
       </c>
       <c r="C246" t="n">
         <v>0.5416666666666666</v>
@@ -3642,7 +3642,7 @@
         </is>
       </c>
       <c r="B247" t="n">
-        <v>0.4062328614550337</v>
+        <v>0.4062329785156162</v>
       </c>
       <c r="C247" t="n">
         <v>0.5416666666666666</v>
@@ -3655,7 +3655,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>0.3987244894861881</v>
+        <v>0.3987246441951566</v>
       </c>
       <c r="C248" t="n">
         <v>0.5208333333333334</v>
@@ -3668,7 +3668,7 @@
         </is>
       </c>
       <c r="B249" t="n">
-        <v>0.3976083064661211</v>
+        <v>0.397608140425685</v>
       </c>
       <c r="C249" t="n">
         <v>0.6041666666666666</v>
@@ -3694,7 +3694,7 @@
         </is>
       </c>
       <c r="B251" t="n">
-        <v>0.3824403102850946</v>
+        <v>0.382440181046291</v>
       </c>
       <c r="C251" t="n">
         <v>0.4791666666666667</v>
@@ -3733,7 +3733,7 @@
         </is>
       </c>
       <c r="B254" t="n">
-        <v>0.3817041043633549</v>
+        <v>0.3817042223029914</v>
       </c>
       <c r="C254" t="n">
         <v>0.5625</v>
@@ -3746,7 +3746,7 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>0.3710146591706711</v>
+        <v>0.3710145067527433</v>
       </c>
       <c r="C255" t="n">
         <v>0.5208333333333334</v>
@@ -3785,7 +3785,7 @@
         </is>
       </c>
       <c r="B258" t="n">
-        <v>0.3516256831994358</v>
+        <v>0.3516257986480986</v>
       </c>
       <c r="C258" t="n">
         <v>0.5416666666666666</v>
@@ -3798,7 +3798,7 @@
         </is>
       </c>
       <c r="B259" t="n">
-        <v>0.3432424087872104</v>
+        <v>0.3432424062782153</v>
       </c>
       <c r="C259" t="n">
         <v>0.5208333333333334</v>
@@ -3811,7 +3811,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>0.3263928638225044</v>
+        <v>0.3263928687686335</v>
       </c>
       <c r="C260" t="n">
         <v>0.5833333333333334</v>
@@ -3837,7 +3837,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>0.3243439600620082</v>
+        <v>0.3243433731467205</v>
       </c>
       <c r="C262" t="n">
         <v>0.5416666666666666</v>
@@ -3889,7 +3889,7 @@
         </is>
       </c>
       <c r="B266" t="n">
-        <v>0.3193310908509726</v>
+        <v>0.3193309790476011</v>
       </c>
       <c r="C266" t="n">
         <v>0.5</v>
@@ -3902,7 +3902,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>0.3089366937930105</v>
+        <v>0.3089366919892413</v>
       </c>
       <c r="C267" t="n">
         <v>0.5208333333333334</v>
@@ -3928,7 +3928,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>0.3037372914797167</v>
+        <v>0.3037370127634409</v>
       </c>
       <c r="C269" t="n">
         <v>0.4583333333333333</v>
@@ -3941,7 +3941,7 @@
         </is>
       </c>
       <c r="B270" t="n">
-        <v>0.2925834624699164</v>
+        <v>0.2925837345745368</v>
       </c>
       <c r="C270" t="n">
         <v>0.5208333333333334</v>
@@ -3967,7 +3967,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>0.2908136541465713</v>
+        <v>0.2908137361060033</v>
       </c>
       <c r="C272" t="n">
         <v>0.5625</v>
@@ -3980,7 +3980,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>0.2899690011378278</v>
+        <v>0.2899692957048656</v>
       </c>
       <c r="C273" t="n">
         <v>0.5208333333333334</v>
@@ -3993,7 +3993,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>0.2869188541310272</v>
+        <v>0.2869190024331554</v>
       </c>
       <c r="C274" t="n">
         <v>0.5416666666666666</v>
@@ -4006,7 +4006,7 @@
         </is>
       </c>
       <c r="B275" t="n">
-        <v>0.2636637511291668</v>
+        <v>0.2636636698149664</v>
       </c>
       <c r="C275" t="n">
         <v>0.5625</v>
@@ -4019,7 +4019,7 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>0.2614895550699656</v>
+        <v>0.2614896235176021</v>
       </c>
       <c r="C276" t="n">
         <v>0.5208333333333334</v>
@@ -4045,7 +4045,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>0.2578193503758046</v>
+        <v>0.2578190922147676</v>
       </c>
       <c r="C278" t="n">
         <v>0.625</v>
@@ -4058,7 +4058,7 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>0.256492199445999</v>
+        <v>0.2564921952997088</v>
       </c>
       <c r="C279" t="n">
         <v>0.6041666666666666</v>
@@ -4071,7 +4071,7 @@
         </is>
       </c>
       <c r="B280" t="n">
-        <v>0.2538878850677768</v>
+        <v>0.2538879678851431</v>
       </c>
       <c r="C280" t="n">
         <v>0.5416666666666666</v>
@@ -4084,7 +4084,7 @@
         </is>
       </c>
       <c r="B281" t="n">
-        <v>0.2513913153135958</v>
+        <v>0.2513913153135963</v>
       </c>
       <c r="C281" t="n">
         <v>0.4583333333333333</v>
@@ -4110,7 +4110,7 @@
         </is>
       </c>
       <c r="B283" t="n">
-        <v>0.2403486572803715</v>
+        <v>0.2403487498185048</v>
       </c>
       <c r="C283" t="n">
         <v>0.5625</v>
@@ -4123,7 +4123,7 @@
         </is>
       </c>
       <c r="B284" t="n">
-        <v>0.2223836223251798</v>
+        <v>0.2223836223251801</v>
       </c>
       <c r="C284" t="n">
         <v>0.5625</v>
@@ -4162,7 +4162,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>0.2149877542306027</v>
+        <v>0.2149875872174312</v>
       </c>
       <c r="C287" t="n">
         <v>0.5416666666666666</v>
@@ -4175,7 +4175,7 @@
         </is>
       </c>
       <c r="B288" t="n">
-        <v>0.2065962247928113</v>
+        <v>0.2065956860687856</v>
       </c>
       <c r="C288" t="n">
         <v>0.4375</v>
@@ -4188,7 +4188,7 @@
         </is>
       </c>
       <c r="B289" t="n">
-        <v>0.2053131524656102</v>
+        <v>0.2053131524656084</v>
       </c>
       <c r="C289" t="n">
         <v>0.5625</v>
@@ -4201,7 +4201,7 @@
         </is>
       </c>
       <c r="B290" t="n">
-        <v>0.1949519927108954</v>
+        <v>0.1949522372614676</v>
       </c>
       <c r="C290" t="n">
         <v>0.5416666666666666</v>
@@ -4214,7 +4214,7 @@
         </is>
       </c>
       <c r="B291" t="n">
-        <v>0.1824852866274511</v>
+        <v>0.1824852866274513</v>
       </c>
       <c r="C291" t="n">
         <v>0.5208333333333334</v>
@@ -4227,7 +4227,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>0.1821491331061249</v>
+        <v>0.1821491308717773</v>
       </c>
       <c r="C292" t="n">
         <v>0.5</v>
@@ -4240,7 +4240,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>0.1810139435325284</v>
+        <v>0.1810140699887457</v>
       </c>
       <c r="C293" t="n">
         <v>0.5416666666666666</v>
@@ -4253,7 +4253,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>0.178597213871011</v>
+        <v>0.1785973128525471</v>
       </c>
       <c r="C294" t="n">
         <v>0.5208333333333334</v>
@@ -4266,7 +4266,7 @@
         </is>
       </c>
       <c r="B295" t="n">
-        <v>0.1733567598564625</v>
+        <v>0.1733566352324376</v>
       </c>
       <c r="C295" t="n">
         <v>0.5625</v>
@@ -4305,7 +4305,7 @@
         </is>
       </c>
       <c r="B298" t="n">
-        <v>0.1574387770887993</v>
+        <v>0.1574384699491556</v>
       </c>
       <c r="C298" t="n">
         <v>0.625</v>
@@ -4318,7 +4318,7 @@
         </is>
       </c>
       <c r="B299" t="n">
-        <v>0.1573486916077915</v>
+        <v>0.1573485743666316</v>
       </c>
       <c r="C299" t="n">
         <v>0.4791666666666667</v>
@@ -4344,7 +4344,7 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>0.1521935195346185</v>
+        <v>0.1521935169071786</v>
       </c>
       <c r="C301" t="n">
         <v>0.5416666666666666</v>
@@ -4357,7 +4357,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>0.1490757126639375</v>
+        <v>0.1490757126639377</v>
       </c>
       <c r="C302" t="n">
         <v>0.4375</v>
@@ -4370,7 +4370,7 @@
         </is>
       </c>
       <c r="B303" t="n">
-        <v>0.1452166518546749</v>
+        <v>0.1452165695324092</v>
       </c>
       <c r="C303" t="n">
         <v>0.5625</v>
@@ -4383,7 +4383,7 @@
         </is>
       </c>
       <c r="B304" t="n">
-        <v>0.1393708249738861</v>
+        <v>0.1393710469384009</v>
       </c>
       <c r="C304" t="n">
         <v>0.625</v>
@@ -4396,7 +4396,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>0.1342653752173639</v>
+        <v>0.1342654623519939</v>
       </c>
       <c r="C305" t="n">
         <v>0.5</v>
@@ -4422,7 +4422,7 @@
         </is>
       </c>
       <c r="B307" t="n">
-        <v>0.1273305391163282</v>
+        <v>0.1273303025017971</v>
       </c>
       <c r="C307" t="n">
         <v>0.4791666666666667</v>
@@ -4435,7 +4435,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>0.1192917403965856</v>
+        <v>0.1192915405892294</v>
       </c>
       <c r="C308" t="n">
         <v>0.5625</v>
@@ -4448,7 +4448,7 @@
         </is>
       </c>
       <c r="B309" t="n">
-        <v>0.1105139385537481</v>
+        <v>0.1105140668697073</v>
       </c>
       <c r="C309" t="n">
         <v>0.6041666666666666</v>
@@ -4461,7 +4461,7 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>0.1027042835263656</v>
+        <v>0.1027041269258329</v>
       </c>
       <c r="C310" t="n">
         <v>0.5208333333333334</v>
@@ -4474,7 +4474,7 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>0.09325623766310276</v>
+        <v>0.093256158929369</v>
       </c>
       <c r="C311" t="n">
         <v>0.5208333333333334</v>
@@ -4513,7 +4513,7 @@
         </is>
       </c>
       <c r="B314" t="n">
-        <v>0.07593724606566843</v>
+        <v>0.07593713426871518</v>
       </c>
       <c r="C314" t="n">
         <v>0.5416666666666666</v>
@@ -4526,7 +4526,7 @@
         </is>
       </c>
       <c r="B315" t="n">
-        <v>0.07267953091471213</v>
+        <v>0.07267941474108852</v>
       </c>
       <c r="C315" t="n">
         <v>0.4583333333333333</v>
@@ -4539,7 +4539,7 @@
         </is>
       </c>
       <c r="B316" t="n">
-        <v>0.06802001306213823</v>
+        <v>0.06802000873936898</v>
       </c>
       <c r="C316" t="n">
         <v>0.5208333333333334</v>
@@ -4565,7 +4565,7 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>0.05700163107154532</v>
+        <v>0.05700144661110063</v>
       </c>
       <c r="C318" t="n">
         <v>0.6041666666666666</v>
@@ -4578,7 +4578,7 @@
         </is>
       </c>
       <c r="B319" t="n">
-        <v>0.05638959605506422</v>
+        <v>0.05638959126193432</v>
       </c>
       <c r="C319" t="n">
         <v>0.6041666666666666</v>
@@ -4591,7 +4591,7 @@
         </is>
       </c>
       <c r="B320" t="n">
-        <v>0.05611233214907152</v>
+        <v>0.05611255091931167</v>
       </c>
       <c r="C320" t="n">
         <v>0.4791666666666667</v>
@@ -4617,7 +4617,7 @@
         </is>
       </c>
       <c r="B322" t="n">
-        <v>0.0507083911780859</v>
+        <v>0.05070838100439179</v>
       </c>
       <c r="C322" t="n">
         <v>0.5833333333333334</v>
@@ -4630,7 +4630,7 @@
         </is>
       </c>
       <c r="B323" t="n">
-        <v>0.04947234736263395</v>
+        <v>0.04947252522842827</v>
       </c>
       <c r="C323" t="n">
         <v>0.5</v>
@@ -4643,7 +4643,7 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>0.04883238564714154</v>
+        <v>0.04883245370349498</v>
       </c>
       <c r="C324" t="n">
         <v>0.5416666666666666</v>
@@ -4656,7 +4656,7 @@
         </is>
       </c>
       <c r="B325" t="n">
-        <v>0.04713555878976905</v>
+        <v>0.047135402133611</v>
       </c>
       <c r="C325" t="n">
         <v>0.5833333333333334</v>
@@ -4682,7 +4682,7 @@
         </is>
       </c>
       <c r="B327" t="n">
-        <v>0.0426937404311436</v>
+        <v>0.04269383414035177</v>
       </c>
       <c r="C327" t="n">
         <v>0.4166666666666667</v>
@@ -4695,7 +4695,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>0.03837022396573175</v>
+        <v>0.03837022343424801</v>
       </c>
       <c r="C328" t="n">
         <v>0.5208333333333334</v>
@@ -4708,7 +4708,7 @@
         </is>
       </c>
       <c r="B329" t="n">
-        <v>0.03184932858211553</v>
+        <v>0.03184953888036679</v>
       </c>
       <c r="C329" t="n">
         <v>0.4375</v>
@@ -4721,7 +4721,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>0.02865150498711677</v>
+        <v>0.02865141808955118</v>
       </c>
       <c r="C330" t="n">
         <v>0.5416666666666666</v>
@@ -4734,7 +4734,7 @@
         </is>
       </c>
       <c r="B331" t="n">
-        <v>0.02522573445963383</v>
+        <v>0.02522565226518814</v>
       </c>
       <c r="C331" t="n">
         <v>0.625</v>
@@ -4760,7 +4760,7 @@
         </is>
       </c>
       <c r="B333" t="n">
-        <v>0.02221816845917624</v>
+        <v>0.02221774775722896</v>
       </c>
       <c r="C333" t="n">
         <v>0.4583333333333333</v>
@@ -4773,7 +4773,7 @@
         </is>
       </c>
       <c r="B334" t="n">
-        <v>0.0178154493963707</v>
+        <v>0.01781556272303542</v>
       </c>
       <c r="C334" t="n">
         <v>0.5625</v>
@@ -4786,7 +4786,7 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>0.01571785283047777</v>
+        <v>0.01571785600808218</v>
       </c>
       <c r="C335" t="n">
         <v>0.5833333333333334</v>
@@ -4799,7 +4799,7 @@
         </is>
       </c>
       <c r="B336" t="n">
-        <v>0.00727990309441795</v>
+        <v>0.007279786599559301</v>
       </c>
       <c r="C336" t="n">
         <v>0.5833333333333334</v>
@@ -4812,7 +4812,7 @@
         </is>
       </c>
       <c r="B337" t="n">
-        <v>0.006047059503627938</v>
+        <v>0.006047060193914433</v>
       </c>
       <c r="C337" t="n">
         <v>0.5625</v>
@@ -4825,7 +4825,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>0.004253817723270936</v>
+        <v>0.004253988721056201</v>
       </c>
       <c r="C338" t="n">
         <v>0.5208333333333334</v>
@@ -4838,7 +4838,7 @@
         </is>
       </c>
       <c r="B339" t="n">
-        <v>0.004060242771491529</v>
+        <v>0.004060043442466688</v>
       </c>
       <c r="C339" t="n">
         <v>0.5</v>
@@ -4877,7 +4877,7 @@
         </is>
       </c>
       <c r="B342" t="n">
-        <v>-0.01720575808843749</v>
+        <v>-0.01720588621431995</v>
       </c>
       <c r="C342" t="n">
         <v>0.5208333333333334</v>
@@ -4903,7 +4903,7 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>-0.03125547326767386</v>
+        <v>-0.0312554732676732</v>
       </c>
       <c r="C344" t="n">
         <v>0.5</v>
@@ -4916,7 +4916,7 @@
         </is>
       </c>
       <c r="B345" t="n">
-        <v>-0.03147518423391094</v>
+        <v>-0.03147518423391182</v>
       </c>
       <c r="C345" t="n">
         <v>0.5208333333333334</v>
@@ -4929,7 +4929,7 @@
         </is>
       </c>
       <c r="B346" t="n">
-        <v>-0.03723042986216274</v>
+        <v>-0.03723050516675319</v>
       </c>
       <c r="C346" t="n">
         <v>0.5625</v>
@@ -4942,7 +4942,7 @@
         </is>
       </c>
       <c r="B347" t="n">
-        <v>-0.04414402127824357</v>
+        <v>-0.04414368296812787</v>
       </c>
       <c r="C347" t="n">
         <v>0.5208333333333334</v>
@@ -4955,7 +4955,7 @@
         </is>
       </c>
       <c r="B348" t="n">
-        <v>-0.05214535807867005</v>
+        <v>-0.05214535226866157</v>
       </c>
       <c r="C348" t="n">
         <v>0.5</v>
@@ -4968,7 +4968,7 @@
         </is>
       </c>
       <c r="B349" t="n">
-        <v>-0.06004620791697013</v>
+        <v>-0.06004642115699832</v>
       </c>
       <c r="C349" t="n">
         <v>0.625</v>
@@ -4981,7 +4981,7 @@
         </is>
       </c>
       <c r="B350" t="n">
-        <v>-0.06226016276236312</v>
+        <v>-0.0622600050987997</v>
       </c>
       <c r="C350" t="n">
         <v>0.5</v>
@@ -4994,7 +4994,7 @@
         </is>
       </c>
       <c r="B351" t="n">
-        <v>-0.06949194715021045</v>
+        <v>-0.06949207816112157</v>
       </c>
       <c r="C351" t="n">
         <v>0.5416666666666666</v>
@@ -5007,7 +5007,7 @@
         </is>
       </c>
       <c r="B352" t="n">
-        <v>-0.07228304065200619</v>
+        <v>-0.07228313968060607</v>
       </c>
       <c r="C352" t="n">
         <v>0.4791666666666667</v>
@@ -5020,7 +5020,7 @@
         </is>
       </c>
       <c r="B353" t="n">
-        <v>-0.07503824266925041</v>
+        <v>-0.07503817860514261</v>
       </c>
       <c r="C353" t="n">
         <v>0.5</v>
@@ -5033,7 +5033,7 @@
         </is>
       </c>
       <c r="B354" t="n">
-        <v>-0.09064952042244068</v>
+        <v>-0.09064952513304481</v>
       </c>
       <c r="C354" t="n">
         <v>0.5208333333333334</v>
@@ -5046,7 +5046,7 @@
         </is>
       </c>
       <c r="B355" t="n">
-        <v>-0.09351931200306074</v>
+        <v>-0.09351922631689824</v>
       </c>
       <c r="C355" t="n">
         <v>0.5</v>
@@ -5059,7 +5059,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>-0.09505430706244822</v>
+        <v>-0.09505420432447154</v>
       </c>
       <c r="C356" t="n">
         <v>0.5208333333333334</v>
@@ -5072,7 +5072,7 @@
         </is>
       </c>
       <c r="B357" t="n">
-        <v>-0.09506587078458129</v>
+        <v>-0.09506597232727887</v>
       </c>
       <c r="C357" t="n">
         <v>0.4791666666666667</v>
@@ -5085,7 +5085,7 @@
         </is>
       </c>
       <c r="B358" t="n">
-        <v>-0.1103340331586474</v>
+        <v>-0.1103340331586476</v>
       </c>
       <c r="C358" t="n">
         <v>0.4791666666666667</v>
@@ -5098,7 +5098,7 @@
         </is>
       </c>
       <c r="B359" t="n">
-        <v>-0.130790994937487</v>
+        <v>-0.1307909942902359</v>
       </c>
       <c r="C359" t="n">
         <v>0.4791666666666667</v>
@@ -5111,7 +5111,7 @@
         </is>
       </c>
       <c r="B360" t="n">
-        <v>-0.1311652156593476</v>
+        <v>-0.131165064484471</v>
       </c>
       <c r="C360" t="n">
         <v>0.5416666666666666</v>
@@ -5124,7 +5124,7 @@
         </is>
       </c>
       <c r="B361" t="n">
-        <v>-0.1516640024745086</v>
+        <v>-0.1516642254105294</v>
       </c>
       <c r="C361" t="n">
         <v>0.5208333333333334</v>
@@ -5163,7 +5163,7 @@
         </is>
       </c>
       <c r="B364" t="n">
-        <v>-0.1665304389236537</v>
+        <v>-0.1665305057648832</v>
       </c>
       <c r="C364" t="n">
         <v>0.375</v>
@@ -5176,7 +5176,7 @@
         </is>
       </c>
       <c r="B365" t="n">
-        <v>-0.1680694187146768</v>
+        <v>-0.1680693626546562</v>
       </c>
       <c r="C365" t="n">
         <v>0.5208333333333334</v>
@@ -5189,7 +5189,7 @@
         </is>
       </c>
       <c r="B366" t="n">
-        <v>-0.1744867338376975</v>
+        <v>-0.1744866571162783</v>
       </c>
       <c r="C366" t="n">
         <v>0.6041666666666666</v>
@@ -5202,7 +5202,7 @@
         </is>
       </c>
       <c r="B367" t="n">
-        <v>-0.1746422443581386</v>
+        <v>-0.1746422443581388</v>
       </c>
       <c r="C367" t="n">
         <v>0.5</v>
@@ -5215,7 +5215,7 @@
         </is>
       </c>
       <c r="B368" t="n">
-        <v>-0.1810427469814109</v>
+        <v>-0.1810428758890091</v>
       </c>
       <c r="C368" t="n">
         <v>0.4375</v>
@@ -5228,7 +5228,7 @@
         </is>
       </c>
       <c r="B369" t="n">
-        <v>-0.1822693580887771</v>
+        <v>-0.1822692568760326</v>
       </c>
       <c r="C369" t="n">
         <v>0.4791666666666667</v>
@@ -5241,7 +5241,7 @@
         </is>
       </c>
       <c r="B370" t="n">
-        <v>-0.1822740468598685</v>
+        <v>-0.1822741131711197</v>
       </c>
       <c r="C370" t="n">
         <v>0.4583333333333333</v>
@@ -5254,7 +5254,7 @@
         </is>
       </c>
       <c r="B371" t="n">
-        <v>-0.1895984806510611</v>
+        <v>-0.1895984101195818</v>
       </c>
       <c r="C371" t="n">
         <v>0.4375</v>
@@ -5267,7 +5267,7 @@
         </is>
       </c>
       <c r="B372" t="n">
-        <v>-0.1914879801948061</v>
+        <v>-0.1914877989475746</v>
       </c>
       <c r="C372" t="n">
         <v>0.4375</v>
@@ -5280,7 +5280,7 @@
         </is>
       </c>
       <c r="B373" t="n">
-        <v>-0.193750821944655</v>
+        <v>-0.1937510609620837</v>
       </c>
       <c r="C373" t="n">
         <v>0.4791666666666667</v>
@@ -5293,7 +5293,7 @@
         </is>
       </c>
       <c r="B374" t="n">
-        <v>-0.1997338438396586</v>
+        <v>-0.199733747156613</v>
       </c>
       <c r="C374" t="n">
         <v>0.5416666666666666</v>
@@ -5306,7 +5306,7 @@
         </is>
       </c>
       <c r="B375" t="n">
-        <v>-0.2076384310551809</v>
+        <v>-0.2076384836546298</v>
       </c>
       <c r="C375" t="n">
         <v>0.625</v>
@@ -5319,7 +5319,7 @@
         </is>
       </c>
       <c r="B376" t="n">
-        <v>-0.2088667251422363</v>
+        <v>-0.2088668341468816</v>
       </c>
       <c r="C376" t="n">
         <v>0.5625</v>
@@ -5332,7 +5332,7 @@
         </is>
       </c>
       <c r="B377" t="n">
-        <v>-0.2093006915714488</v>
+        <v>-0.2093006915714489</v>
       </c>
       <c r="C377" t="n">
         <v>0.4583333333333333</v>
@@ -5358,7 +5358,7 @@
         </is>
       </c>
       <c r="B379" t="n">
-        <v>-0.2113704059298119</v>
+        <v>-0.2113704634842489</v>
       </c>
       <c r="C379" t="n">
         <v>0.375</v>
@@ -5371,7 +5371,7 @@
         </is>
       </c>
       <c r="B380" t="n">
-        <v>-0.2176300649699374</v>
+        <v>-0.2176300070186311</v>
       </c>
       <c r="C380" t="n">
         <v>0.5208333333333334</v>
@@ -5384,7 +5384,7 @@
         </is>
       </c>
       <c r="B381" t="n">
-        <v>-0.2277646343487085</v>
+        <v>-0.2277646343487086</v>
       </c>
       <c r="C381" t="n">
         <v>0.5208333333333334</v>
@@ -5436,7 +5436,7 @@
         </is>
       </c>
       <c r="B385" t="n">
-        <v>-0.2526419305058666</v>
+        <v>-0.2526420162030711</v>
       </c>
       <c r="C385" t="n">
         <v>0.5</v>
@@ -5462,7 +5462,7 @@
         </is>
       </c>
       <c r="B387" t="n">
-        <v>-0.2606968483096863</v>
+        <v>-0.260696906471196</v>
       </c>
       <c r="C387" t="n">
         <v>0.5416666666666666</v>
@@ -5501,7 +5501,7 @@
         </is>
       </c>
       <c r="B390" t="n">
-        <v>-0.2875606449853529</v>
+        <v>-0.2875606461839871</v>
       </c>
       <c r="C390" t="n">
         <v>0.5</v>
@@ -5514,7 +5514,7 @@
         </is>
       </c>
       <c r="B391" t="n">
-        <v>-0.2925479316070733</v>
+        <v>-0.2925479919418209</v>
       </c>
       <c r="C391" t="n">
         <v>0.5208333333333334</v>
@@ -5527,7 +5527,7 @@
         </is>
       </c>
       <c r="B392" t="n">
-        <v>-0.3022513238145279</v>
+        <v>-0.3022512841776727</v>
       </c>
       <c r="C392" t="n">
         <v>0.5</v>
@@ -5540,7 +5540,7 @@
         </is>
       </c>
       <c r="B393" t="n">
-        <v>-0.3041680205282238</v>
+        <v>-0.3041679544575415</v>
       </c>
       <c r="C393" t="n">
         <v>0.5208333333333334</v>
@@ -5553,7 +5553,7 @@
         </is>
       </c>
       <c r="B394" t="n">
-        <v>-0.308576310659238</v>
+        <v>-0.3085762333308468</v>
       </c>
       <c r="C394" t="n">
         <v>0.5</v>
@@ -5566,7 +5566,7 @@
         </is>
       </c>
       <c r="B395" t="n">
-        <v>-0.3128807196177726</v>
+        <v>-0.3128804298756889</v>
       </c>
       <c r="C395" t="n">
         <v>0.5208333333333334</v>
@@ -5579,7 +5579,7 @@
         </is>
       </c>
       <c r="B396" t="n">
-        <v>-0.3130493455217482</v>
+        <v>-0.3130493019971295</v>
       </c>
       <c r="C396" t="n">
         <v>0.5416666666666666</v>
@@ -5592,7 +5592,7 @@
         </is>
       </c>
       <c r="B397" t="n">
-        <v>-0.315502776285108</v>
+        <v>-0.3155027154447072</v>
       </c>
       <c r="C397" t="n">
         <v>0.5</v>
@@ -5605,7 +5605,7 @@
         </is>
       </c>
       <c r="B398" t="n">
-        <v>-0.3329546010707395</v>
+        <v>-0.332954602166767</v>
       </c>
       <c r="C398" t="n">
         <v>0.4791666666666667</v>
@@ -5631,7 +5631,7 @@
         </is>
       </c>
       <c r="B400" t="n">
-        <v>-0.342220546435384</v>
+        <v>-0.3422205888958231</v>
       </c>
       <c r="C400" t="n">
         <v>0.4375</v>
@@ -5644,7 +5644,7 @@
         </is>
       </c>
       <c r="B401" t="n">
-        <v>-0.3433004175899786</v>
+        <v>-0.3433004671499481</v>
       </c>
       <c r="C401" t="n">
         <v>0.4375</v>
@@ -5657,7 +5657,7 @@
         </is>
       </c>
       <c r="B402" t="n">
-        <v>-0.3528576965501299</v>
+        <v>-0.3528577449922465</v>
       </c>
       <c r="C402" t="n">
         <v>0.5625</v>
@@ -5670,7 +5670,7 @@
         </is>
       </c>
       <c r="B403" t="n">
-        <v>-0.3537961945675199</v>
+        <v>-0.3537963159376378</v>
       </c>
       <c r="C403" t="n">
         <v>0.5</v>
@@ -5683,7 +5683,7 @@
         </is>
       </c>
       <c r="B404" t="n">
-        <v>-0.3543315809272172</v>
+        <v>-0.3543314643945094</v>
       </c>
       <c r="C404" t="n">
         <v>0.5625</v>
@@ -5722,7 +5722,7 @@
         </is>
       </c>
       <c r="B407" t="n">
-        <v>-0.3807579760167503</v>
+        <v>-0.3807578842103522</v>
       </c>
       <c r="C407" t="n">
         <v>0.5625</v>
@@ -5735,7 +5735,7 @@
         </is>
       </c>
       <c r="B408" t="n">
-        <v>-0.3814875859143263</v>
+        <v>-0.3814876748750027</v>
       </c>
       <c r="C408" t="n">
         <v>0.4791666666666667</v>
@@ -5761,7 +5761,7 @@
         </is>
       </c>
       <c r="B410" t="n">
-        <v>-0.3894540442373022</v>
+        <v>-0.3894540442373021</v>
       </c>
       <c r="C410" t="n">
         <v>0.5833333333333334</v>
@@ -5774,7 +5774,7 @@
         </is>
       </c>
       <c r="B411" t="n">
-        <v>-0.4067045714088646</v>
+        <v>-0.4067046283376468</v>
       </c>
       <c r="C411" t="n">
         <v>0.3958333333333333</v>
@@ -5787,7 +5787,7 @@
         </is>
       </c>
       <c r="B412" t="n">
-        <v>-0.4122074556903389</v>
+        <v>-0.4122072697365675</v>
       </c>
       <c r="C412" t="n">
         <v>0.5208333333333334</v>
@@ -5800,7 +5800,7 @@
         </is>
       </c>
       <c r="B413" t="n">
-        <v>-0.4129799554817046</v>
+        <v>-0.4129798992570536</v>
       </c>
       <c r="C413" t="n">
         <v>0.5</v>
@@ -5813,7 +5813,7 @@
         </is>
       </c>
       <c r="B414" t="n">
-        <v>-0.4143196522051774</v>
+        <v>-0.4143196920636917</v>
       </c>
       <c r="C414" t="n">
         <v>0.5625</v>
@@ -5826,7 +5826,7 @@
         </is>
       </c>
       <c r="B415" t="n">
-        <v>-0.4166977436574946</v>
+        <v>-0.4166977786485623</v>
       </c>
       <c r="C415" t="n">
         <v>0.5</v>
@@ -5839,7 +5839,7 @@
         </is>
       </c>
       <c r="B416" t="n">
-        <v>-0.4223693260907987</v>
+        <v>-0.4223694597433535</v>
       </c>
       <c r="C416" t="n">
         <v>0.4166666666666667</v>
@@ -5852,7 +5852,7 @@
         </is>
       </c>
       <c r="B417" t="n">
-        <v>-0.4274041544527734</v>
+        <v>-0.4274042122194746</v>
       </c>
       <c r="C417" t="n">
         <v>0.4375</v>
@@ -5865,7 +5865,7 @@
         </is>
       </c>
       <c r="B418" t="n">
-        <v>-0.433466490239638</v>
+        <v>-0.4334665259056286</v>
       </c>
       <c r="C418" t="n">
         <v>0.4583333333333333</v>
@@ -5878,7 +5878,7 @@
         </is>
       </c>
       <c r="B419" t="n">
-        <v>-0.4346238626432494</v>
+        <v>-0.4346239059630449</v>
       </c>
       <c r="C419" t="n">
         <v>0.4375</v>
@@ -5891,7 +5891,7 @@
         </is>
       </c>
       <c r="B420" t="n">
-        <v>-0.4409726421120681</v>
+        <v>-0.4409726443942943</v>
       </c>
       <c r="C420" t="n">
         <v>0.4583333333333333</v>
@@ -5904,7 +5904,7 @@
         </is>
       </c>
       <c r="B421" t="n">
-        <v>-0.443640968083032</v>
+        <v>-0.443640968354135</v>
       </c>
       <c r="C421" t="n">
         <v>0.4791666666666667</v>
@@ -5917,7 +5917,7 @@
         </is>
       </c>
       <c r="B422" t="n">
-        <v>-0.450019448048161</v>
+        <v>-0.4500194480481605</v>
       </c>
       <c r="C422" t="n">
         <v>0.4375</v>
@@ -5930,7 +5930,7 @@
         </is>
       </c>
       <c r="B423" t="n">
-        <v>-0.4507662375005699</v>
+        <v>-0.450766173122864</v>
       </c>
       <c r="C423" t="n">
         <v>0.5</v>
@@ -5943,7 +5943,7 @@
         </is>
       </c>
       <c r="B424" t="n">
-        <v>-0.4545890358205383</v>
+        <v>-0.4545891279952733</v>
       </c>
       <c r="C424" t="n">
         <v>0.5</v>
@@ -5956,7 +5956,7 @@
         </is>
       </c>
       <c r="B425" t="n">
-        <v>-0.4564343439478648</v>
+        <v>-0.4564343439478655</v>
       </c>
       <c r="C425" t="n">
         <v>0.5208333333333334</v>
@@ -5969,7 +5969,7 @@
         </is>
       </c>
       <c r="B426" t="n">
-        <v>-0.4591147524700627</v>
+        <v>-0.4591146856553394</v>
       </c>
       <c r="C426" t="n">
         <v>0.5</v>
@@ -5982,7 +5982,7 @@
         </is>
       </c>
       <c r="B427" t="n">
-        <v>-0.46316199233026</v>
+        <v>-0.463161926533571</v>
       </c>
       <c r="C427" t="n">
         <v>0.5208333333333334</v>
@@ -5995,7 +5995,7 @@
         </is>
       </c>
       <c r="B428" t="n">
-        <v>-0.4646281733944898</v>
+        <v>-0.4646280994326325</v>
       </c>
       <c r="C428" t="n">
         <v>0.5208333333333334</v>
@@ -6021,7 +6021,7 @@
         </is>
       </c>
       <c r="B430" t="n">
-        <v>-0.4690103042967398</v>
+        <v>-0.4690102647464794</v>
       </c>
       <c r="C430" t="n">
         <v>0.4375</v>
@@ -6047,7 +6047,7 @@
         </is>
       </c>
       <c r="B432" t="n">
-        <v>-0.4766289282318513</v>
+        <v>-0.4766289283771269</v>
       </c>
       <c r="C432" t="n">
         <v>0.4583333333333333</v>
@@ -6060,7 +6060,7 @@
         </is>
       </c>
       <c r="B433" t="n">
-        <v>-0.4817040480622802</v>
+        <v>-0.4817040180568929</v>
       </c>
       <c r="C433" t="n">
         <v>0.5625</v>
@@ -6086,7 +6086,7 @@
         </is>
       </c>
       <c r="B435" t="n">
-        <v>-0.4871697529880155</v>
+        <v>-0.487169873673577</v>
       </c>
       <c r="C435" t="n">
         <v>0.5416666666666666</v>
@@ -6099,7 +6099,7 @@
         </is>
       </c>
       <c r="B436" t="n">
-        <v>-0.4884036396621115</v>
+        <v>-0.4884037052050213</v>
       </c>
       <c r="C436" t="n">
         <v>0.4375</v>
@@ -6125,7 +6125,7 @@
         </is>
       </c>
       <c r="B438" t="n">
-        <v>-0.4964724756975573</v>
+        <v>-0.4964724315161874</v>
       </c>
       <c r="C438" t="n">
         <v>0.5</v>
@@ -6138,7 +6138,7 @@
         </is>
       </c>
       <c r="B439" t="n">
-        <v>-0.5022569374647321</v>
+        <v>-0.5022569749289608</v>
       </c>
       <c r="C439" t="n">
         <v>0.4791666666666667</v>
@@ -6151,7 +6151,7 @@
         </is>
       </c>
       <c r="B440" t="n">
-        <v>-0.5060463890525972</v>
+        <v>-0.5060463303840018</v>
       </c>
       <c r="C440" t="n">
         <v>0.5208333333333334</v>
@@ -6177,7 +6177,7 @@
         </is>
       </c>
       <c r="B442" t="n">
-        <v>-0.5123666947753773</v>
+        <v>-0.5123666513176651</v>
       </c>
       <c r="C442" t="n">
         <v>0.4166666666666667</v>
@@ -6190,7 +6190,7 @@
         </is>
       </c>
       <c r="B443" t="n">
-        <v>-0.5130368626701858</v>
+        <v>-0.5130368616631336</v>
       </c>
       <c r="C443" t="n">
         <v>0.4375</v>
@@ -6203,7 +6203,7 @@
         </is>
       </c>
       <c r="B444" t="n">
-        <v>-0.5147123302138972</v>
+        <v>-0.514712391177238</v>
       </c>
       <c r="C444" t="n">
         <v>0.5</v>
@@ -6242,7 +6242,7 @@
         </is>
       </c>
       <c r="B447" t="n">
-        <v>-0.5408430187609004</v>
+        <v>-0.5408430183653874</v>
       </c>
       <c r="C447" t="n">
         <v>0.4583333333333333</v>
@@ -6255,7 +6255,7 @@
         </is>
       </c>
       <c r="B448" t="n">
-        <v>-0.5461865716532237</v>
+        <v>-0.5461864227531704</v>
       </c>
       <c r="C448" t="n">
         <v>0.3958333333333333</v>
@@ -6281,7 +6281,7 @@
         </is>
       </c>
       <c r="B450" t="n">
-        <v>-0.5512564006599481</v>
+        <v>-0.5512564410418312</v>
       </c>
       <c r="C450" t="n">
         <v>0.5</v>
@@ -6294,7 +6294,7 @@
         </is>
       </c>
       <c r="B451" t="n">
-        <v>-0.5711522978562333</v>
+        <v>-0.5711523005937764</v>
       </c>
       <c r="C451" t="n">
         <v>0.5208333333333334</v>
@@ -6307,7 +6307,7 @@
         </is>
       </c>
       <c r="B452" t="n">
-        <v>-0.582253185299588</v>
+        <v>-0.5822532105923472</v>
       </c>
       <c r="C452" t="n">
         <v>0.3958333333333333</v>
@@ -6333,7 +6333,7 @@
         </is>
       </c>
       <c r="B454" t="n">
-        <v>-0.5856207517296341</v>
+        <v>-0.5856207534568457</v>
       </c>
       <c r="C454" t="n">
         <v>0.4791666666666667</v>
@@ -6359,7 +6359,7 @@
         </is>
       </c>
       <c r="B456" t="n">
-        <v>-0.5915645285015929</v>
+        <v>-0.5915644863582528</v>
       </c>
       <c r="C456" t="n">
         <v>0.4791666666666667</v>
@@ -6385,7 +6385,7 @@
         </is>
       </c>
       <c r="B458" t="n">
-        <v>-0.5951695718530257</v>
+        <v>-0.5951695486473004</v>
       </c>
       <c r="C458" t="n">
         <v>0.4583333333333333</v>
@@ -6398,7 +6398,7 @@
         </is>
       </c>
       <c r="B459" t="n">
-        <v>-0.5966080972964849</v>
+        <v>-0.5966080959964872</v>
       </c>
       <c r="C459" t="n">
         <v>0.4791666666666667</v>
@@ -6437,7 +6437,7 @@
         </is>
       </c>
       <c r="B462" t="n">
-        <v>-0.6044059005815811</v>
+        <v>-0.6044059517005677</v>
       </c>
       <c r="C462" t="n">
         <v>0.5416666666666666</v>
@@ -6450,7 +6450,7 @@
         </is>
       </c>
       <c r="B463" t="n">
-        <v>-0.6078092020226886</v>
+        <v>-0.6078093271747592</v>
       </c>
       <c r="C463" t="n">
         <v>0.4791666666666667</v>
@@ -6463,7 +6463,7 @@
         </is>
       </c>
       <c r="B464" t="n">
-        <v>-0.6105172461417414</v>
+        <v>-0.6105172775107525</v>
       </c>
       <c r="C464" t="n">
         <v>0.5</v>
@@ -6541,7 +6541,7 @@
         </is>
       </c>
       <c r="B470" t="n">
-        <v>-0.6533724187632588</v>
+        <v>-0.6533724393827139</v>
       </c>
       <c r="C470" t="n">
         <v>0.5625</v>
@@ -6554,7 +6554,7 @@
         </is>
       </c>
       <c r="B471" t="n">
-        <v>-0.6583684501268716</v>
+        <v>-0.6583684255579617</v>
       </c>
       <c r="C471" t="n">
         <v>0.5416666666666666</v>
@@ -6580,7 +6580,7 @@
         </is>
       </c>
       <c r="B473" t="n">
-        <v>-0.6688338869736525</v>
+        <v>-0.6688339076565257</v>
       </c>
       <c r="C473" t="n">
         <v>0.5625</v>
@@ -6593,7 +6593,7 @@
         </is>
       </c>
       <c r="B474" t="n">
-        <v>-0.6709077019955217</v>
+        <v>-0.6709077425304846</v>
       </c>
       <c r="C474" t="n">
         <v>0.5</v>
@@ -6619,7 +6619,7 @@
         </is>
       </c>
       <c r="B476" t="n">
-        <v>-0.6946755398916467</v>
+        <v>-0.6946755862305283</v>
       </c>
       <c r="C476" t="n">
         <v>0.4583333333333333</v>
@@ -6632,7 +6632,7 @@
         </is>
       </c>
       <c r="B477" t="n">
-        <v>-0.6964986124918063</v>
+        <v>-0.6964985913415053</v>
       </c>
       <c r="C477" t="n">
         <v>0.4375</v>
@@ -6645,7 +6645,7 @@
         </is>
       </c>
       <c r="B478" t="n">
-        <v>-0.6987585743665549</v>
+        <v>-0.6987586312114591</v>
       </c>
       <c r="C478" t="n">
         <v>0.5</v>
@@ -6684,7 +6684,7 @@
         </is>
       </c>
       <c r="B481" t="n">
-        <v>-0.7168517196684805</v>
+        <v>-0.7168517071262732</v>
       </c>
       <c r="C481" t="n">
         <v>0.3958333333333333</v>
@@ -6697,7 +6697,7 @@
         </is>
       </c>
       <c r="B482" t="n">
-        <v>-0.7264067233112046</v>
+        <v>-0.7264067233112045</v>
       </c>
       <c r="C482" t="n">
         <v>0.4375</v>
@@ -6736,7 +6736,7 @@
         </is>
       </c>
       <c r="B485" t="n">
-        <v>-0.7789549042526169</v>
+        <v>-0.7789548805220738</v>
       </c>
       <c r="C485" t="n">
         <v>0.5</v>
@@ -6749,7 +6749,7 @@
         </is>
       </c>
       <c r="B486" t="n">
-        <v>-0.7837991358371772</v>
+        <v>-0.7837991135547892</v>
       </c>
       <c r="C486" t="n">
         <v>0.5416666666666666</v>
@@ -6775,7 +6775,7 @@
         </is>
       </c>
       <c r="B488" t="n">
-        <v>-0.7926624033272314</v>
+        <v>-0.7926623851742882</v>
       </c>
       <c r="C488" t="n">
         <v>0.4791666666666667</v>
@@ -6814,7 +6814,7 @@
         </is>
       </c>
       <c r="B491" t="n">
-        <v>-0.826741736522965</v>
+        <v>-0.8267417081315316</v>
       </c>
       <c r="C491" t="n">
         <v>0.5416666666666666</v>
@@ -6840,7 +6840,7 @@
         </is>
       </c>
       <c r="B493" t="n">
-        <v>-0.8579574108800347</v>
+        <v>-0.8579574108800349</v>
       </c>
       <c r="C493" t="n">
         <v>0.6041666666666666</v>
@@ -6853,7 +6853,7 @@
         </is>
       </c>
       <c r="B494" t="n">
-        <v>-0.8955032137234921</v>
+        <v>-0.8955031938368361</v>
       </c>
       <c r="C494" t="n">
         <v>0.4166666666666667</v>
@@ -6879,7 +6879,7 @@
         </is>
       </c>
       <c r="B496" t="n">
-        <v>-0.928734438685121</v>
+        <v>-0.9287344387395559</v>
       </c>
       <c r="C496" t="n">
         <v>0.3958333333333333</v>
@@ -6905,7 +6905,7 @@
         </is>
       </c>
       <c r="B498" t="n">
-        <v>-0.9434905113143552</v>
+        <v>-0.9434905171215312</v>
       </c>
       <c r="C498" t="n">
         <v>0.4166666666666667</v>
@@ -6918,7 +6918,7 @@
         </is>
       </c>
       <c r="B499" t="n">
-        <v>-0.9461735702179312</v>
+        <v>-0.9461735654832581</v>
       </c>
       <c r="C499" t="n">
         <v>0.4375</v>
@@ -6931,7 +6931,7 @@
         </is>
       </c>
       <c r="B500" t="n">
-        <v>-0.957138658350877</v>
+        <v>-0.9571386624994924</v>
       </c>
       <c r="C500" t="n">
         <v>0.3958333333333333</v>

</xml_diff>